<commit_message>
Mejoras en la creación de hoja de excel
</commit_message>
<xml_diff>
--- a/DepreciationDBApp.Presentation/bin/Debug/net5.0-windows/myexcel.xlsx
+++ b/DepreciationDBApp.Presentation/bin/Debug/net5.0-windows/myexcel.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R88563d02e3984155"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R3fc4db70e0dd4f32"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <x:si>
     <x:t>Nombre del Activo</x:t>
   </x:si>
@@ -26,28 +26,46 @@
     <x:t>DNI del empleado</x:t>
   </x:si>
   <x:si>
-    <x:t>Televisor</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jaime</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C3Qe7o22</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0011106</x:t>
+    <x:t>Descripción del Activo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Valor del activo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vida util</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Descripción</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PC gamer ultima generación</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kevin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SflpybZh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>002</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fonts count="3">
+  <x:fonts count="4">
     <x:font>
       <x:sz val="11"/>
       <x:color theme="1"/>
       <x:name val="Calibri"/>
       <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
     </x:font>
     <x:font>
       <x:b/>
@@ -59,12 +77,24 @@
       <x:color theme="1"/>
     </x:font>
   </x:fonts>
-  <x:fills count="2">
+  <x:fills count="4">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFFF00"/>
+        <x:bgColor rgb="FF000000"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray0625">
+        <x:fgColor rgb="FFFFFF00"/>
+        <x:bgColor rgb="FF000000"/>
+      </x:patternFill>
     </x:fill>
   </x:fills>
   <x:borders count="1">
@@ -79,17 +109,20 @@
   <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </x:cellStyleXfs>
-  <x:cellXfs count="5">
+  <x:cellXfs count="6">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <x:alignment horizontal="left" vertical="center"/>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <x:alignment horizontal="center"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <x:alignment horizontal="left" vertical="center"/>
+      <x:alignment horizontal="center"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <x:alignment horizontal="left" vertical="center"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <x:alignment horizontal="center"/>
     </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
@@ -385,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="B2:E3"/>
+  <x:dimension ref="B2:E10"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -397,32 +430,61 @@
     <x:col min="5" max="5" width="23" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="2" s="1" customFormat="1">
-      <x:c r="B2" s="4" t="s">
+    <x:row r="2">
+      <x:c r="B2" s="3" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="C2" s="4" t="s">
+      <x:c r="C2" s="3" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="D2" s="4" t="s">
+      <x:c r="D2" s="3" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="E2" s="4" t="s">
+      <x:c r="E2" s="3" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
       <x:c r="B3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="E3" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" ht="15" customHeight="1">
+      <x:c r="B6" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="C3" t="s">
+    </x:row>
+    <x:row r="8">
+      <x:c r="B8" s="1" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D3" t="s">
+      <x:c r="C8" s="5">
+        <x:v>56000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9">
+      <x:c r="B9" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="E3" t="s">
+      <x:c r="C9" s="5">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10">
+      <x:c r="B10" s="1" t="s">
         <x:v>7</x:v>
+      </x:c>
+      <x:c r="C10" s="5" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Cambio en el cuerpo del mensaje enviado y bordes de celdas ...
</commit_message>
<xml_diff>
--- a/DepreciationDBApp.Presentation/bin/Debug/net5.0-windows/myexcel.xlsx
+++ b/DepreciationDBApp.Presentation/bin/Debug/net5.0-windows/myexcel.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R3fc4db70e0dd4f32"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R04c40fb2849d4144"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -38,26 +38,26 @@
     <x:t>Descripción</x:t>
   </x:si>
   <x:si>
-    <x:t>PC gamer ultima generación</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PC</x:t>
+    <x:t>Monitor 4K</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Monitor</x:t>
   </x:si>
   <x:si>
     <x:t>Kevin</x:t>
   </x:si>
   <x:si>
-    <x:t>SflpybZh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>002</x:t>
+    <x:t>vybDy162</x:t>
+  </x:si>
+  <x:si>
+    <x:t>001</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fonts count="4">
+  <x:fonts count="5">
     <x:font>
       <x:sz val="11"/>
       <x:color theme="1"/>
@@ -69,6 +69,10 @@
     </x:font>
     <x:font>
       <x:b/>
+      <x:color theme="1"/>
+    </x:font>
+    <x:font>
+      <x:b/>
       <x:sz val="16"/>
     </x:font>
     <x:font>
@@ -77,7 +81,7 @@
       <x:color theme="1"/>
     </x:font>
   </x:fonts>
-  <x:fills count="4">
+  <x:fills count="3">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
@@ -90,14 +94,8 @@
         <x:bgColor rgb="FF000000"/>
       </x:patternFill>
     </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray0625">
-        <x:fgColor rgb="FFFFFF00"/>
-        <x:bgColor rgb="FF000000"/>
-      </x:patternFill>
-    </x:fill>
   </x:fills>
-  <x:borders count="1">
+  <x:borders count="2">
     <x:border>
       <x:left/>
       <x:right/>
@@ -105,17 +103,33 @@
       <x:bottom/>
       <x:diagonal/>
     </x:border>
+    <x:border>
+      <x:left style="thin">
+        <x:color rgb="FF808080"/>
+      </x:left>
+      <x:right style="thin">
+        <x:color rgb="FF808080"/>
+      </x:right>
+      <x:top style="thin">
+        <x:color rgb="FF808080"/>
+      </x:top>
+      <x:bottom style="thin">
+        <x:color rgb="FF808080"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
   </x:borders>
   <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </x:cellStyleXfs>
-  <x:cellXfs count="6">
+  <x:cellXfs count="7">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <x:xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -431,16 +445,16 @@
   </x:cols>
   <x:sheetData>
     <x:row r="2">
-      <x:c r="B2" s="3" t="s">
+      <x:c r="B2" s="4" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="C2" s="3" t="s">
+      <x:c r="C2" s="4" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="D2" s="3" t="s">
+      <x:c r="D2" s="4" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="E2" s="3" t="s">
+      <x:c r="E2" s="4" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
@@ -458,32 +472,32 @@
         <x:v>12</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" ht="15" customHeight="1">
-      <x:c r="B6" s="1" t="s">
+    <x:row r="6">
+      <x:c r="B6" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
-      <x:c r="B8" s="1" t="s">
+      <x:c r="B8" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="C8" s="5">
-        <x:v>56000</x:v>
+      <x:c r="C8" s="6">
+        <x:v>5000</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
-      <x:c r="B9" s="1" t="s">
+      <x:c r="B9" s="2" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C9" s="5">
-        <x:v>5</x:v>
+      <x:c r="C9" s="6">
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
-      <x:c r="B10" s="1" t="s">
+      <x:c r="B10" s="2" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="C10" s="5" t="s">
+      <x:c r="C10" s="6" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>

</xml_diff>